<commit_message>
[GEN MAIN] SCH & PCB update
</commit_message>
<xml_diff>
--- a/2_LF_Generator_Main/1_Schematic/Plasma_LF_Generator_Main_V1.0_BOM.xlsx
+++ b/2_LF_Generator_Main/1_Schematic/Plasma_LF_Generator_Main_V1.0_BOM.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Work\20171211_Femto_LF Gen\0_GitHub_Data_LF\2_LF_Generator_Main\1_Schematic\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LF_Generator_Main_V1.0_SCH_2018" sheetId="1" r:id="rId1"/>
@@ -18,12 +13,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">LF_Generator_Main_V1.0_SCH_2018!$B$5:$M$5</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="267">
   <si>
     <t>No</t>
   </si>
@@ -85,9 +80,6 @@
     <t>26.0x10.0</t>
   </si>
   <si>
-    <t>F472Z2KV</t>
-  </si>
-  <si>
     <t>F472Z2kV</t>
   </si>
   <si>
@@ -143,9 +135,6 @@
   </si>
   <si>
     <t>12.95000mm</t>
-  </si>
-  <si>
-    <t>KMHVN227M2G</t>
   </si>
   <si>
     <t>220uF/400V</t>
@@ -824,6 +813,22 @@
   </si>
   <si>
     <t>LF-1116</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>F472Z2KV</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>GBU610</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>AL-CAP_D5.0_2.0PITCH</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>KMHVN227M2G</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -1637,7 +1642,7 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1702,6 +1707,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1806,7 +1814,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1841,7 +1849,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2018,7 +2026,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2028,8 +2036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2050,7 +2058,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2092,31 +2100,31 @@
         <v>10</v>
       </c>
       <c r="M5" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="O5" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="P5" s="7" t="s">
         <v>251</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="Q5" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="R5" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="Q5" s="7" t="s">
+      <c r="S5" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="R5" s="7" t="s">
+      <c r="T5" s="8" t="s">
         <v>255</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="U5" s="7" t="s">
         <v>256</v>
-      </c>
-      <c r="T5" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="U5" s="7" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -2127,7 +2135,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>13</v>
@@ -2173,33 +2181,33 @@
       <c r="B7" s="12">
         <v>2</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="E7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>23</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>24</v>
       </c>
       <c r="H7" s="13">
         <v>2</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J7" s="13">
         <v>0</v>
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M7" s="13">
         <v>100</v>
@@ -2220,33 +2228,33 @@
       <c r="B8" s="12">
         <v>3</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="G8" s="18" t="s">
         <v>29</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>30</v>
       </c>
       <c r="H8" s="13">
         <v>1</v>
       </c>
       <c r="I8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>32</v>
       </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M8" s="13">
         <v>100</v>
@@ -2267,35 +2275,35 @@
       <c r="B9" s="12">
         <v>4</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="E9" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="G9" s="13" t="s">
         <v>36</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>37</v>
       </c>
       <c r="H9" s="13">
         <v>3</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9" s="13">
         <v>0</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L9" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
@@ -2315,34 +2323,34 @@
         <v>5</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>40</v>
+        <v>266</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>40</v>
+        <v>266</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="H10" s="13">
         <v>2</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J10" s="13">
         <v>0</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L10" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
@@ -2362,34 +2370,34 @@
         <v>6</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>43</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>45</v>
       </c>
       <c r="H11" s="13">
         <v>7</v>
       </c>
       <c r="I11" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J11" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="J11" s="13" t="s">
-        <v>48</v>
-      </c>
       <c r="K11" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L11" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M11" s="13">
         <v>10</v>
@@ -2411,34 +2419,34 @@
         <v>7</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E12" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>43</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>45</v>
       </c>
       <c r="H12" s="13">
         <v>2</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L12" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M12" s="13">
         <v>10</v>
@@ -2460,32 +2468,32 @@
         <v>8</v>
       </c>
       <c r="C13" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="13" t="s">
+      <c r="G13" s="13" t="s">
         <v>52</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>54</v>
       </c>
       <c r="H13" s="13">
         <v>2</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J13" s="13">
         <v>0</v>
       </c>
       <c r="K13" s="13"/>
       <c r="L13" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M13" s="13">
         <v>70</v>
@@ -2507,32 +2515,32 @@
         <v>9</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H14" s="13">
         <v>2</v>
       </c>
       <c r="I14" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="13" t="s">
-        <v>61</v>
-      </c>
       <c r="K14" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="M14" s="13">
         <v>800</v>
@@ -2554,32 +2562,32 @@
         <v>10</v>
       </c>
       <c r="C15" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="13" t="s">
         <v>62</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>64</v>
       </c>
       <c r="F15" s="13">
         <v>330</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H15" s="13">
         <v>2</v>
       </c>
       <c r="I15" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="J15" s="13" t="s">
         <v>66</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="K15" s="13"/>
       <c r="L15" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M15" s="13">
         <v>10</v>
@@ -2601,32 +2609,32 @@
         <v>11</v>
       </c>
       <c r="C16" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="F16" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>71</v>
       </c>
       <c r="H16" s="13">
         <v>3</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K16" s="13"/>
       <c r="L16" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M16" s="13">
         <v>10</v>
@@ -2648,32 +2656,32 @@
         <v>12</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F17" s="13">
         <v>10</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H17" s="13">
         <v>2</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K17" s="13"/>
       <c r="L17" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M17" s="13">
         <v>10</v>
@@ -2695,32 +2703,32 @@
         <v>13</v>
       </c>
       <c r="C18" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="F18" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="13" t="s">
         <v>78</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>80</v>
       </c>
       <c r="H18" s="13">
         <v>4</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K18" s="13"/>
       <c r="L18" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M18" s="13">
         <v>10</v>
@@ -2742,32 +2750,32 @@
         <v>14</v>
       </c>
       <c r="C19" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>84</v>
-      </c>
       <c r="G19" s="13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H19" s="13">
         <v>2</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K19" s="13"/>
       <c r="L19" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M19" s="13">
         <v>10</v>
@@ -2789,32 +2797,32 @@
         <v>15</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D20" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="13" t="s">
         <v>87</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>89</v>
       </c>
       <c r="H20" s="13">
         <v>2</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K20" s="13"/>
       <c r="L20" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M20" s="13">
         <v>10</v>
@@ -2836,32 +2844,32 @@
         <v>16</v>
       </c>
       <c r="C21" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="F21" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="13" t="s">
         <v>91</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>93</v>
       </c>
       <c r="H21" s="13">
         <v>2</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K21" s="13"/>
       <c r="L21" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M21" s="13">
         <v>10</v>
@@ -2883,34 +2891,34 @@
         <v>17</v>
       </c>
       <c r="C22" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F22" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E22" s="13" t="s">
+      <c r="G22" s="13" t="s">
         <v>96</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>98</v>
       </c>
       <c r="H22" s="13">
         <v>1</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L22" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M22" s="13">
         <v>10</v>
@@ -2932,32 +2940,32 @@
         <v>18</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D23" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="13" t="s">
         <v>101</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>103</v>
       </c>
       <c r="H23" s="13">
         <v>1</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="K23" s="13"/>
       <c r="L23" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M23" s="13">
         <v>10</v>
@@ -2979,34 +2987,34 @@
         <v>19</v>
       </c>
       <c r="C24" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="E24" s="13" t="s">
+      <c r="G24" s="13" t="s">
         <v>106</v>
-      </c>
-      <c r="F24" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>108</v>
       </c>
       <c r="H24" s="13">
         <v>1</v>
       </c>
       <c r="I24" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K24" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="L24" s="13" t="s">
         <v>109</v>
-      </c>
-      <c r="J24" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="K24" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="L24" s="13" t="s">
-        <v>111</v>
       </c>
       <c r="M24" s="13"/>
       <c r="N24" s="13"/>
@@ -3026,32 +3034,32 @@
         <v>20</v>
       </c>
       <c r="C25" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="F25" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" s="13" t="s">
         <v>113</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>115</v>
       </c>
       <c r="H25" s="13">
         <v>1</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K25" s="13"/>
       <c r="L25" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M25" s="13">
         <v>10</v>
@@ -3073,32 +3081,32 @@
         <v>21</v>
       </c>
       <c r="C26" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="F26" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G26" s="13" t="s">
         <v>117</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>119</v>
       </c>
       <c r="H26" s="13">
         <v>1</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K26" s="13"/>
       <c r="L26" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M26" s="13">
         <v>10</v>
@@ -3120,32 +3128,32 @@
         <v>22</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D27" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G27" s="13" t="s">
         <v>121</v>
-      </c>
-      <c r="E27" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>123</v>
       </c>
       <c r="H27" s="13">
         <v>1</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K27" s="13"/>
       <c r="L27" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M27" s="13">
         <v>80</v>
@@ -3167,23 +3175,23 @@
         <v>23</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E28" s="18"/>
       <c r="F28" s="18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H28" s="13">
         <v>1</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="J28" s="13">
         <v>0</v>
@@ -3210,32 +3218,32 @@
         <v>24</v>
       </c>
       <c r="C29" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G29" s="13" t="s">
         <v>129</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="E29" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>131</v>
       </c>
       <c r="H29" s="13">
         <v>2</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="J29" s="13">
         <v>0</v>
       </c>
       <c r="K29" s="13"/>
       <c r="L29" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M29" s="13">
         <v>30</v>
@@ -3257,32 +3265,32 @@
         <v>25</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H30" s="13">
         <v>2</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="J30" s="13">
         <v>0</v>
       </c>
       <c r="K30" s="13"/>
       <c r="L30" s="13" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M30" s="13">
         <v>30</v>
@@ -3303,26 +3311,26 @@
       <c r="B31" s="12">
         <v>26</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="19" t="s">
+        <v>264</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="G31" s="13" t="s">
         <v>137</v>
-      </c>
-      <c r="D31" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>139</v>
       </c>
       <c r="H31" s="13">
         <v>1</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J31" s="13">
         <v>0</v>
@@ -3349,34 +3357,34 @@
         <v>27</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D32" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G32" s="13" t="s">
         <v>141</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="F32" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>143</v>
       </c>
       <c r="H32" s="13">
         <v>1</v>
       </c>
       <c r="I32" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="K32" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="L32" s="13" t="s">
         <v>144</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="K32" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="L32" s="13" t="s">
-        <v>146</v>
       </c>
       <c r="M32" s="13">
         <v>70</v>
@@ -3398,34 +3406,34 @@
         <v>28</v>
       </c>
       <c r="C33" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="G33" s="13" t="s">
         <v>148</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>150</v>
       </c>
       <c r="H33" s="13">
         <v>2</v>
       </c>
       <c r="I33" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="L33" s="13" t="s">
         <v>151</v>
-      </c>
-      <c r="J33" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="K33" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="L33" s="13" t="s">
-        <v>153</v>
       </c>
       <c r="M33" s="13">
         <v>180</v>
@@ -3447,34 +3455,34 @@
         <v>29</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="H34" s="13">
         <v>2</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K34" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="L34" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M34" s="13">
         <v>200</v>
@@ -3496,34 +3504,34 @@
         <v>30</v>
       </c>
       <c r="C35" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="G35" s="13" t="s">
         <v>159</v>
-      </c>
-      <c r="D35" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="E35" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="F35" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>161</v>
       </c>
       <c r="H35" s="13">
         <v>2</v>
       </c>
       <c r="I35" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="J35" s="13" t="s">
         <v>162</v>
       </c>
-      <c r="J35" s="13" t="s">
-        <v>164</v>
-      </c>
       <c r="K35" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="L35" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="M35" s="13">
         <v>3380</v>
@@ -3545,34 +3553,34 @@
         <v>31</v>
       </c>
       <c r="C36" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="E36" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="F36" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="G36" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="E36" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="F36" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>168</v>
       </c>
       <c r="H36" s="13">
         <v>2</v>
       </c>
       <c r="I36" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="K36" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="L36" s="13" t="s">
         <v>169</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>172</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="L36" s="13" t="s">
-        <v>171</v>
       </c>
       <c r="M36" s="13">
         <v>3640</v>
@@ -3594,34 +3602,34 @@
         <v>32</v>
       </c>
       <c r="C37" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="E37" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="F37" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="G37" s="13" t="s">
         <v>174</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="G37" s="13" t="s">
-        <v>176</v>
       </c>
       <c r="H37" s="13">
         <v>1</v>
       </c>
       <c r="I37" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="J37" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="L37" s="13" t="s">
         <v>177</v>
-      </c>
-      <c r="J37" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="K37" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="L37" s="13" t="s">
-        <v>179</v>
       </c>
       <c r="M37" s="13">
         <v>750</v>
@@ -3643,34 +3651,34 @@
         <v>33</v>
       </c>
       <c r="C38" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="E38" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="F38" s="13" t="s">
+        <v>180</v>
+      </c>
+      <c r="G38" s="13" t="s">
         <v>182</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>183</v>
-      </c>
-      <c r="F38" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>184</v>
       </c>
       <c r="H38" s="13">
         <v>1</v>
       </c>
       <c r="I38" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="J38" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="J38" s="13" t="s">
-        <v>187</v>
-      </c>
       <c r="K38" s="13" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L38" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="M38" s="13">
         <v>2850</v>
@@ -3692,34 +3700,34 @@
         <v>34</v>
       </c>
       <c r="C39" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="E39" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="D39" s="13" t="s">
+      <c r="F39" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="G39" s="13" t="s">
         <v>189</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="F39" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>191</v>
       </c>
       <c r="H39" s="13">
         <v>1</v>
       </c>
       <c r="I39" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="J39" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="J39" s="13" t="s">
-        <v>194</v>
-      </c>
       <c r="K39" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L39" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="M39" s="13">
         <v>2850</v>
@@ -3741,34 +3749,34 @@
         <v>35</v>
       </c>
       <c r="C40" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E40" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="F40" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="G40" s="13" t="s">
         <v>196</v>
-      </c>
-      <c r="E40" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="F40" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="G40" s="13" t="s">
-        <v>198</v>
       </c>
       <c r="H40" s="13">
         <v>14</v>
       </c>
       <c r="I40" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="J40" s="13" t="s">
         <v>199</v>
       </c>
-      <c r="J40" s="13" t="s">
-        <v>201</v>
-      </c>
       <c r="K40" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L40" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M40" s="13">
         <v>120</v>
@@ -3790,34 +3798,34 @@
         <v>36</v>
       </c>
       <c r="C41" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="E41" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="F41" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="G41" s="13" t="s">
         <v>203</v>
-      </c>
-      <c r="E41" s="13" t="s">
-        <v>204</v>
-      </c>
-      <c r="F41" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>205</v>
       </c>
       <c r="H41" s="13">
         <v>1</v>
       </c>
       <c r="I41" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="J41" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="J41" s="13" t="s">
-        <v>208</v>
-      </c>
       <c r="K41" s="13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="L41" s="13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="M41" s="13">
         <v>250</v>
@@ -3839,34 +3847,34 @@
         <v>37</v>
       </c>
       <c r="C42" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>208</v>
+      </c>
+      <c r="E42" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="F42" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="E42" s="13" t="s">
+      <c r="G42" s="13" t="s">
         <v>211</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="G42" s="13" t="s">
-        <v>213</v>
       </c>
       <c r="H42" s="13">
         <v>2</v>
       </c>
       <c r="I42" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="J42" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="K42" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="L42" s="13" t="s">
         <v>214</v>
-      </c>
-      <c r="J42" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="K42" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="L42" s="13" t="s">
-        <v>216</v>
       </c>
       <c r="M42" s="13">
         <v>1200</v>
@@ -3888,34 +3896,34 @@
         <v>38</v>
       </c>
       <c r="C43" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H43" s="13">
         <v>1</v>
       </c>
       <c r="I43" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="J43" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="J43" s="13" t="s">
-        <v>222</v>
-      </c>
       <c r="K43" s="13" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="L43" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M43" s="13">
         <v>120</v>
@@ -3937,34 +3945,34 @@
         <v>39</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D44" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="G44" s="13" t="s">
         <v>196</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="G44" s="13" t="s">
-        <v>198</v>
       </c>
       <c r="H44" s="13">
         <v>1</v>
       </c>
       <c r="I44" s="13" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J44" s="13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="K44" s="13" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="L44" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M44" s="13">
         <v>120</v>
@@ -3986,34 +3994,34 @@
         <v>40</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="H45" s="13">
         <v>2</v>
       </c>
       <c r="I45" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="J45" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="J45" s="13" t="s">
-        <v>229</v>
-      </c>
       <c r="K45" s="13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L45" s="13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M45" s="13"/>
       <c r="N45" s="13"/>
@@ -4033,34 +4041,34 @@
         <v>41</v>
       </c>
       <c r="C46" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="G46" s="13" t="s">
         <v>230</v>
-      </c>
-      <c r="D46" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="E46" s="13" t="s">
-        <v>231</v>
-      </c>
-      <c r="F46" s="13" t="s">
-        <v>230</v>
-      </c>
-      <c r="G46" s="13" t="s">
-        <v>232</v>
       </c>
       <c r="H46" s="13">
         <v>1</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J46" s="13" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K46" s="13" t="s">
         <v>18</v>
       </c>
       <c r="L46" s="13" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="M46" s="13">
         <v>20800</v>
@@ -4082,25 +4090,25 @@
         <v>42</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="H47" s="13">
         <v>2</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J47" s="13">
         <v>0</v>
@@ -4127,25 +4135,25 @@
         <v>43</v>
       </c>
       <c r="C48" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="E48" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="F48" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="G48" s="13" t="s">
         <v>239</v>
-      </c>
-      <c r="E48" s="13" t="s">
-        <v>240</v>
-      </c>
-      <c r="F48" s="13" t="s">
-        <v>239</v>
-      </c>
-      <c r="G48" s="13" t="s">
-        <v>241</v>
       </c>
       <c r="H48" s="13">
         <v>1</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J48" s="13">
         <v>0</v>
@@ -4172,34 +4180,34 @@
         <v>44</v>
       </c>
       <c r="C49" s="20" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E49" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="G49" s="16" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="H49" s="16">
         <v>1</v>
       </c>
       <c r="I49" s="16" t="s">
+        <v>243</v>
+      </c>
+      <c r="J49" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="J49" s="16" t="s">
-        <v>247</v>
-      </c>
       <c r="K49" s="16" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L49" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="M49" s="16">
         <v>500</v>
@@ -4215,7 +4223,7 @@
     </row>
     <row r="51" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B51" s="1" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -4228,10 +4236,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:D18"/>
+  <dimension ref="B5:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -4311,7 +4319,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>22.5</v>
       </c>
@@ -4322,7 +4330,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18">
         <f>B17/2</f>
         <v>11.25</v>
@@ -4334,6 +4342,121 @@
       <c r="D18">
         <f>D17/2</f>
         <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F21">
+        <v>4.83</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>22.5</v>
+      </c>
+      <c r="C22">
+        <v>10.5</v>
+      </c>
+      <c r="D22">
+        <v>4.5</v>
+      </c>
+      <c r="F22">
+        <v>5.33</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <f>B22/2</f>
+        <v>11.25</v>
+      </c>
+      <c r="C23">
+        <f>C22/2</f>
+        <v>5.25</v>
+      </c>
+      <c r="D23">
+        <f>D22/2</f>
+        <v>2.25</v>
+      </c>
+      <c r="F23">
+        <f>SUM(F21:F22)</f>
+        <v>10.16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F24">
+        <f>F23/2</f>
+        <v>5.08</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>22.3</v>
+      </c>
+      <c r="E25">
+        <v>3.56</v>
+      </c>
+      <c r="F25">
+        <f>F24/2</f>
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <f>D25/2</f>
+        <v>11.15</v>
+      </c>
+      <c r="E26">
+        <f>E25/2</f>
+        <v>1.78</v>
+      </c>
+      <c r="F26">
+        <f>SUM(F24:F25)</f>
+        <v>7.62</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>10.9</v>
+      </c>
+      <c r="D28">
+        <v>2.54</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <f>B28/2</f>
+        <v>5.45</v>
+      </c>
+      <c r="D29">
+        <f>D28/2</f>
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <f>B29-1</f>
+        <v>4.45</v>
+      </c>
+      <c r="D30">
+        <f>SUM(D28:D29)</f>
+        <v>3.81</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>9.65</v>
+      </c>
+      <c r="D33">
+        <v>6.35</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <f>C33/2</f>
+        <v>4.8250000000000002</v>
+      </c>
+      <c r="D34">
+        <f>D33/2</f>
+        <v>3.1749999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[GEN MAIN]Sch & PCB uudate
</commit_message>
<xml_diff>
--- a/2_LF_Generator_Main/1_Schematic/Plasma_LF_Generator_Main_V1.0_BOM.xlsx
+++ b/2_LF_Generator_Main/1_Schematic/Plasma_LF_Generator_Main_V1.0_BOM.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My_Work\20171211_Femto_LF Gen\0_GitHub_Data_LF\2_LF_Generator_Main\1_Schematic\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="120" windowWidth="28035" windowHeight="12105"/>
   </bookViews>
   <sheets>
     <sheet name="LF_Generator_Main_V1.0_SCH" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">LF_Generator_Main_V1.0_SCH!$B$4:$L$4</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="280">
   <si>
     <t>No</t>
   </si>
@@ -112,733 +118,763 @@
     <t>0.1uF/630VDC</t>
   </si>
   <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C-1608</t>
+  </si>
+  <si>
+    <t>0.1uF</t>
+  </si>
+  <si>
+    <t>MURATA</t>
+  </si>
+  <si>
+    <t>GCM188R71H104KA57J</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>C6,C9,C12,C13,C24,C25</t>
+  </si>
+  <si>
+    <t>0.95mm</t>
+  </si>
+  <si>
+    <t>1.6x0.8</t>
+  </si>
+  <si>
+    <t>TDAVN227M2G</t>
+  </si>
+  <si>
+    <t>SAMYOUNG</t>
+  </si>
+  <si>
+    <t>220uF/400V</t>
+  </si>
+  <si>
+    <t>ALUMINUM CAPACITORS, TDA(KMG) Series D30.0mm</t>
+  </si>
+  <si>
+    <t>C7,C8</t>
+  </si>
+  <si>
+    <t>30.0mm</t>
+  </si>
+  <si>
+    <t>D30.0mm</t>
+  </si>
+  <si>
+    <t>2.2uF</t>
+  </si>
+  <si>
+    <t>GRT188R61H225ME13D</t>
+  </si>
+  <si>
+    <t>CAP CER 2.2UF 50V X5R 0603</t>
+  </si>
+  <si>
+    <t>C10,C14,C15,C16,C19,C20,C21,C22,C26</t>
+  </si>
+  <si>
+    <t>0.022uF</t>
+  </si>
+  <si>
+    <t>SAMSUNG</t>
+  </si>
+  <si>
+    <t>CL10B223JB8NNNC</t>
+  </si>
+  <si>
+    <t>CAP CER 0.022UF 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>C11,C23</t>
+  </si>
+  <si>
+    <t>ECW-FD2J225K</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>2.2uF/630VDC</t>
+  </si>
+  <si>
+    <t>Metallized Polyester Film Capacitor 2.2UF 630VDC</t>
+  </si>
+  <si>
+    <t>C17,C18</t>
+  </si>
+  <si>
+    <t>17.7mm</t>
+  </si>
+  <si>
+    <t>ECWFD2J</t>
+  </si>
+  <si>
+    <t>25.3xx12.4</t>
+  </si>
+  <si>
+    <t>R-1608</t>
+  </si>
+  <si>
+    <t>WR06X3300FTL</t>
+  </si>
+  <si>
+    <t>WALSIN</t>
+  </si>
+  <si>
+    <t>RES SMD 330 OHM 5% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R1,R18</t>
+  </si>
+  <si>
+    <t>0.40mm</t>
+  </si>
+  <si>
+    <t>WR06X1001FTL</t>
+  </si>
+  <si>
+    <t>1K</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R2,R3,R14</t>
+  </si>
+  <si>
+    <t>WR06X1002FTL</t>
+  </si>
+  <si>
+    <t>10K</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R4,R15</t>
+  </si>
+  <si>
+    <t>MFR-50J-10R</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>10 / 0.5W</t>
+  </si>
+  <si>
+    <t>Metal film resistor 10 0.5W 5%, 300V</t>
+  </si>
+  <si>
+    <t>R5,R6</t>
+  </si>
+  <si>
+    <t>3.3mm</t>
+  </si>
+  <si>
+    <t>MFR-1/2W</t>
+  </si>
+  <si>
+    <t>9.0x3.3</t>
+  </si>
+  <si>
+    <t>MFR-25J-10K</t>
+  </si>
+  <si>
+    <t>10K / 0.25W</t>
+  </si>
+  <si>
+    <t>Metal film resistor 10K, 0.25W,5%, 250V</t>
+  </si>
+  <si>
+    <t>R7,R8,R19</t>
+  </si>
+  <si>
+    <t>2.4mm</t>
+  </si>
+  <si>
+    <t>MFR-1/4W</t>
+  </si>
+  <si>
+    <t>6.4x2.4</t>
+  </si>
+  <si>
+    <t>MFR-2W</t>
+  </si>
+  <si>
+    <t>MFR200</t>
+  </si>
+  <si>
+    <t>150K / 2W</t>
+  </si>
+  <si>
+    <t>Metal Oxide film resistor 150K, 2W, 5%, 350V</t>
+  </si>
+  <si>
+    <t>R9,R10,R11,R12</t>
+  </si>
+  <si>
+    <t>5.0mm</t>
+  </si>
+  <si>
+    <t>15.5x5.0</t>
+  </si>
+  <si>
+    <t>WR06X4701FTL</t>
+  </si>
+  <si>
+    <t>4.7K</t>
+  </si>
+  <si>
+    <t>RES SMD 4.7K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R13,R23</t>
+  </si>
+  <si>
+    <t>WR06X2001FTL</t>
+  </si>
+  <si>
+    <t>2K</t>
+  </si>
+  <si>
+    <t>RES SMD 2K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>MFR-50J-1M</t>
+  </si>
+  <si>
+    <t>1M / 0.5W</t>
+  </si>
+  <si>
+    <t>Metal film resistor 1M, 0.5W 5%, 300V</t>
+  </si>
+  <si>
+    <t>R20</t>
+  </si>
+  <si>
+    <t>3296W-503-LF</t>
+  </si>
+  <si>
+    <t>BOURNS</t>
+  </si>
+  <si>
+    <t>VR 5K</t>
+  </si>
+  <si>
+    <t>Potentiometers 5K LINEAR 10% DIP-3</t>
+  </si>
+  <si>
+    <t>R21</t>
+  </si>
+  <si>
+    <t>11.55mm</t>
+  </si>
+  <si>
+    <t>PTV09A-4015U-B103</t>
+  </si>
+  <si>
+    <t>9.53x4.83</t>
+  </si>
+  <si>
+    <t>WR06X3001FTL</t>
+  </si>
+  <si>
+    <t>3K</t>
+  </si>
+  <si>
+    <t>RES SMD 3K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R24</t>
+  </si>
+  <si>
+    <t>NTC_10D-11</t>
+  </si>
+  <si>
+    <t>NTC 10D-11</t>
+  </si>
+  <si>
+    <t>SAMKYUNG</t>
+  </si>
+  <si>
+    <t>Power Thermistor 10ohm 45sec</t>
+  </si>
+  <si>
+    <t>RT1</t>
+  </si>
+  <si>
+    <t>17.5mm</t>
+  </si>
+  <si>
+    <t>12.5x7.5</t>
+  </si>
+  <si>
+    <t>LF-1116</t>
+  </si>
+  <si>
+    <t>HYUPSIN</t>
+  </si>
+  <si>
+    <t>LINEFILTER f=120HZ L:20mH, Pin size AC10mm/BD:10mm CD:13mm Tolerance¡¾20%</t>
+  </si>
+  <si>
+    <t>LF1</t>
+  </si>
+  <si>
+    <t>21.0mm</t>
+  </si>
+  <si>
+    <t>17.0x17.0</t>
+  </si>
+  <si>
+    <t>1N4740A</t>
+  </si>
+  <si>
+    <t>Onsemi</t>
+  </si>
+  <si>
+    <t>Zener Diode Vz=10V Izsm=454mA 1W 5% DO-41</t>
+  </si>
+  <si>
+    <t>D1,D2</t>
+  </si>
+  <si>
+    <t>2.6mm</t>
+  </si>
+  <si>
+    <t>DO-204AL_DO-41</t>
+  </si>
+  <si>
+    <t>4.1x2.6</t>
+  </si>
+  <si>
+    <t>1N4744A</t>
+  </si>
+  <si>
+    <t>Zener Diode Vz=15V Izsm=304mA 1W 5% DO-41</t>
+  </si>
+  <si>
+    <t>D3,D4</t>
+  </si>
+  <si>
+    <t>GBU610</t>
+  </si>
+  <si>
+    <t>LITEON Semi</t>
+  </si>
+  <si>
+    <t>GLASS PASSIVATED BRIDGE RECTIFIERS</t>
+  </si>
+  <si>
+    <t>D5</t>
+  </si>
+  <si>
+    <t>21.25mm</t>
+  </si>
+  <si>
+    <t>22.3x3.56</t>
+  </si>
+  <si>
+    <t>BR-FH1</t>
+  </si>
+  <si>
+    <t>BEE-RYONG</t>
+  </si>
+  <si>
+    <t>Fuse holder DIP</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>10.3mm</t>
+  </si>
+  <si>
+    <t>24.5x9.8</t>
+  </si>
+  <si>
+    <t>MMBT3904</t>
+  </si>
+  <si>
+    <t>NPN General-Purpose Amplifier 200mA 40V SOT-23</t>
+  </si>
+  <si>
+    <t>Q1,Q2</t>
+  </si>
+  <si>
+    <t>1.2mm</t>
+  </si>
+  <si>
+    <t>2.92x2.40</t>
+  </si>
+  <si>
+    <t>MMBT3906</t>
+  </si>
+  <si>
+    <t>PNP General-Purpose Amplifier 200mA 40V SOT-23</t>
+  </si>
+  <si>
+    <t>Q3,Q4</t>
+  </si>
+  <si>
+    <t>1.20mm</t>
+  </si>
+  <si>
+    <t>FDL100N50F</t>
+  </si>
+  <si>
+    <t>On-Semi</t>
+  </si>
+  <si>
+    <t>MOSFET N-CH 500V 100A TO-264</t>
+  </si>
+  <si>
+    <t>Q5,Q6</t>
+  </si>
+  <si>
+    <t>5.2mm</t>
+  </si>
+  <si>
+    <t>26.4x20.2</t>
+  </si>
+  <si>
+    <t>HCPL-3120-360E</t>
+  </si>
+  <si>
+    <t>AVAGO</t>
+  </si>
+  <si>
+    <t>2.5 Amp Output Current IGBT Gate Drive Optocoupler SMT</t>
+  </si>
+  <si>
+    <t>U1,U2</t>
+  </si>
+  <si>
+    <t>3.56mm</t>
+  </si>
+  <si>
+    <t>9.65x10.9</t>
+  </si>
+  <si>
+    <t>MAX3232CSE</t>
+  </si>
+  <si>
+    <t>MAXIM</t>
+  </si>
+  <si>
+    <t>3.0V to 5.5V, Low-Power, up to 1Mbps, True RS-232 Transceivers Using Four 0.1?iF External Capacitors</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>1.75mm</t>
+  </si>
+  <si>
+    <t>MAX3232ESE</t>
+  </si>
+  <si>
+    <t>10x6.2</t>
+  </si>
+  <si>
+    <t>CAS_6-NP</t>
+  </si>
+  <si>
+    <t>CAS 6-NP</t>
+  </si>
+  <si>
+    <t>LEM</t>
+  </si>
+  <si>
+    <t>5V, 6A Current sensor</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>16mm</t>
+  </si>
+  <si>
+    <t>21.91x13.4</t>
+  </si>
+  <si>
+    <t>LM393M</t>
+  </si>
+  <si>
+    <t>On Semi</t>
+  </si>
+  <si>
+    <t>IC COMPARATOR DUAL DIFF 8-SOP</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>6.2x5.0</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>HOLE4.0MM</t>
+  </si>
+  <si>
+    <t>H1,H2,H3,H4,H5,H6</t>
+  </si>
+  <si>
+    <t>HEADER_2.54MM_1X2</t>
+  </si>
+  <si>
+    <t>HEADER_2.54mm_1x2</t>
+  </si>
+  <si>
+    <t>Anyvendor</t>
+  </si>
+  <si>
+    <t>2.54mm Pitch Pin Header 1x2 T=11.5mm</t>
+  </si>
+  <si>
+    <t>J1,J7,J8,J13,J14,J15,J16,J17</t>
+  </si>
+  <si>
+    <t>11.5mm</t>
+  </si>
+  <si>
+    <t>5.38x2.5</t>
+  </si>
+  <si>
+    <t>DSBU-9PIN</t>
+  </si>
+  <si>
+    <t>DSBU-9PIN-R/A</t>
+  </si>
+  <si>
+    <t>MOLEX</t>
+  </si>
+  <si>
+    <t>D-SUB PCB 2-row 9-pin Female Right angle</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>12.5mm</t>
+  </si>
+  <si>
+    <t>30.8x18.2</t>
+  </si>
+  <si>
+    <t>HEADER_SOCKET_20X2</t>
+  </si>
+  <si>
+    <t>HEADER_SOCKET_2.0mm_2x20</t>
+  </si>
+  <si>
+    <t>Any Vendor</t>
+  </si>
+  <si>
+    <t>2.0mm Pitch Header Socket 2x20 Straight</t>
+  </si>
+  <si>
+    <t>J9,J10</t>
+  </si>
+  <si>
+    <t>4.3mm</t>
+  </si>
+  <si>
+    <t>40.5x4.5</t>
+  </si>
+  <si>
+    <t>5273-06A</t>
+  </si>
+  <si>
+    <t>CON 6-pin, 3.96mm Pitch Throgh hole</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>13.85mm</t>
+  </si>
+  <si>
+    <t>23.0x10.2</t>
+  </si>
+  <si>
+    <t>CON2</t>
+  </si>
+  <si>
+    <t>12512WS-04B</t>
+  </si>
+  <si>
+    <t>YEONHO</t>
+  </si>
+  <si>
+    <t>CON 4-pin, Throgh hole  type</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>4.2mm</t>
+  </si>
+  <si>
+    <t>7.5x3.6</t>
+  </si>
+  <si>
+    <t>5268-04</t>
+  </si>
+  <si>
+    <t>CON Pin-4, 2.5mm pitch Right Angle</t>
+  </si>
+  <si>
+    <t>P3,P4</t>
+  </si>
+  <si>
+    <t>4.9mm</t>
+  </si>
+  <si>
+    <t>12.4x7.9</t>
+  </si>
+  <si>
+    <t>FST10-5FFM</t>
+  </si>
+  <si>
+    <t>Power Plaza</t>
+  </si>
+  <si>
+    <t>67KHz 5V, 15V AC-DC converter 0.13A@220VAC</t>
+  </si>
+  <si>
+    <t>SMPS</t>
+  </si>
+  <si>
+    <t>LM3671MF-3.3</t>
+  </si>
+  <si>
+    <t>58.0x45.0</t>
+  </si>
+  <si>
+    <t>78604/9MC</t>
+  </si>
+  <si>
+    <t>General Purpose Pulse Transformers 10mH 2:1 SMT</t>
+  </si>
+  <si>
+    <t>TX1,TX2</t>
+  </si>
+  <si>
+    <t>6.35mm</t>
+  </si>
+  <si>
+    <t>12.7x9.0</t>
+  </si>
+  <si>
+    <t>High frequency transformer 1:5</t>
+  </si>
+  <si>
+    <t>TX3</t>
+  </si>
+  <si>
+    <t>MOV-14D471K</t>
+  </si>
+  <si>
+    <t>Metal Oxide Varistor Vmax=330VAC, 14mm radial</t>
+  </si>
+  <si>
+    <t>Z1</t>
+  </si>
+  <si>
+    <t>20mm</t>
+  </si>
+  <si>
+    <t>16.5x5.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Part Type Report1 for LF_Generator_Main_V1.0_SCH.sch on 2018-05-07 오전 12:38:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Design Part Type count: 36</t>
+  </si>
+  <si>
+    <t>Unit Cost</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>구매 Cost</t>
+  </si>
+  <si>
+    <t>필요수량</t>
+  </si>
+  <si>
+    <t>MOQ</t>
+  </si>
+  <si>
+    <t>구매수량</t>
+  </si>
+  <si>
+    <t>구매금액</t>
+  </si>
+  <si>
+    <t>ICBanQ</t>
+  </si>
+  <si>
     <t>0.1uF 630VDC Metallized Polyester Film Capacitor</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C-1005</t>
-  </si>
-  <si>
-    <t>14.0x8.5</t>
-  </si>
-  <si>
-    <t>C-1608</t>
-  </si>
-  <si>
-    <t>0.1uF</t>
-  </si>
-  <si>
-    <t>MURATA</t>
-  </si>
-  <si>
-    <t>GCM188R71H104KA57J</t>
-  </si>
-  <si>
-    <t>CAP CER 0.1UF 50V X7R 0603</t>
-  </si>
-  <si>
-    <t>C6,C9,C12,C13,C24,C25</t>
-  </si>
-  <si>
-    <t>0.95mm</t>
-  </si>
-  <si>
-    <t>1.6x0.8</t>
-  </si>
-  <si>
-    <t>TDAVN227M2G</t>
-  </si>
-  <si>
-    <t>SAMYOUNG</t>
-  </si>
-  <si>
-    <t>220uF/400V</t>
-  </si>
-  <si>
-    <t>ALUMINUM CAPACITORS, TDA(KMG) Series D30.0mm</t>
-  </si>
-  <si>
-    <t>C7,C8</t>
-  </si>
-  <si>
-    <t>30.0mm</t>
-  </si>
-  <si>
-    <t>D30.0mm</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
-    <t>GRT188R61H225ME13D</t>
-  </si>
-  <si>
-    <t>CAP CER 2.2UF 50V X5R 0603</t>
-  </si>
-  <si>
-    <t>C10,C14,C15,C16,C19,C20,C21,C22,C26</t>
-  </si>
-  <si>
-    <t>0.022uF</t>
-  </si>
-  <si>
-    <t>SAMSUNG</t>
-  </si>
-  <si>
-    <t>CL10B223JB8NNNC</t>
-  </si>
-  <si>
-    <t>CAP CER 0.022UF 50V X7R 0603</t>
-  </si>
-  <si>
-    <t>C11,C23</t>
-  </si>
-  <si>
-    <t>ECW-FD2J225K</t>
-  </si>
-  <si>
-    <t>Panasonic</t>
-  </si>
-  <si>
-    <t>2.2uF/630VDC</t>
-  </si>
-  <si>
-    <t>Metallized Polyester Film Capacitor 2.2UF 630VDC</t>
-  </si>
-  <si>
-    <t>C17,C18</t>
-  </si>
-  <si>
-    <t>17.7mm</t>
-  </si>
-  <si>
-    <t>ECWFD2J</t>
-  </si>
-  <si>
-    <t>25.3xx12.4</t>
-  </si>
-  <si>
-    <t>R-1608</t>
-  </si>
-  <si>
-    <t>WR06X3300FTL</t>
-  </si>
-  <si>
-    <t>WALSIN</t>
-  </si>
-  <si>
-    <t>RES SMD 330 OHM 5% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R1,R18</t>
-  </si>
-  <si>
-    <t>0.40mm</t>
-  </si>
-  <si>
-    <t>WR06X1001FTL</t>
-  </si>
-  <si>
-    <t>1K</t>
-  </si>
-  <si>
-    <t>RES SMD 1K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R2,R3,R14</t>
-  </si>
-  <si>
-    <t>WR06X1002FTL</t>
-  </si>
-  <si>
-    <t>10K</t>
-  </si>
-  <si>
-    <t>RES SMD 10K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R4,R15</t>
-  </si>
-  <si>
-    <t>MFR-50J-10R</t>
-  </si>
-  <si>
-    <t>YAGEO</t>
-  </si>
-  <si>
-    <t>10 / 0.5W</t>
-  </si>
-  <si>
-    <t>Metal film resistor 10 0.5W 5%, 300V</t>
-  </si>
-  <si>
-    <t>R5,R6</t>
-  </si>
-  <si>
-    <t>3.3mm</t>
-  </si>
-  <si>
-    <t>MFR-1/2W</t>
-  </si>
-  <si>
-    <t>9.0x3.3</t>
-  </si>
-  <si>
-    <t>MFR-25J-10K</t>
-  </si>
-  <si>
-    <t>10K / 0.25W</t>
-  </si>
-  <si>
-    <t>Metal film resistor 10K, 0.25W,5%, 250V</t>
-  </si>
-  <si>
-    <t>R7,R8,R19</t>
-  </si>
-  <si>
-    <t>2.4mm</t>
-  </si>
-  <si>
-    <t>MFR-1/4W</t>
-  </si>
-  <si>
-    <t>6.4x2.4</t>
-  </si>
-  <si>
-    <t>MFR-2W</t>
-  </si>
-  <si>
-    <t>MFR200</t>
-  </si>
-  <si>
-    <t>150K / 2W</t>
-  </si>
-  <si>
-    <t>Metal Oxide film resistor 150K, 2W, 5%, 350V</t>
-  </si>
-  <si>
-    <t>R9,R10,R11,R12</t>
-  </si>
-  <si>
-    <t>5.0mm</t>
-  </si>
-  <si>
-    <t>15.5x5.0</t>
-  </si>
-  <si>
-    <t>WR06X4701FTL</t>
-  </si>
-  <si>
-    <t>4.7K</t>
-  </si>
-  <si>
-    <t>RES SMD 4.7K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R13,R23</t>
-  </si>
-  <si>
-    <t>WR06X2001FTL</t>
-  </si>
-  <si>
-    <t>2K</t>
-  </si>
-  <si>
-    <t>RES SMD 2K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>MFR-50J-1M</t>
-  </si>
-  <si>
-    <t>1M / 0.5W</t>
-  </si>
-  <si>
-    <t>Metal film resistor 1M, 0.5W 5%, 300V</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>3296W-503-LF</t>
-  </si>
-  <si>
-    <t>BOURNS</t>
-  </si>
-  <si>
-    <t>VR 5K</t>
-  </si>
-  <si>
-    <t>Potentiometers 5K LINEAR 10% DIP-3</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>11.55mm</t>
-  </si>
-  <si>
-    <t>PTV09A-4015U-B103</t>
-  </si>
-  <si>
-    <t>9.53x4.83</t>
-  </si>
-  <si>
-    <t>WR06X3001FTL</t>
-  </si>
-  <si>
-    <t>3K</t>
-  </si>
-  <si>
-    <t>RES SMD 3K OHM 1% 1/10W 0603</t>
-  </si>
-  <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>NTC_10D-11</t>
-  </si>
-  <si>
-    <t>NTC 10D-11</t>
-  </si>
-  <si>
-    <t>SAMKYUNG</t>
-  </si>
-  <si>
-    <t>Power Thermistor 10ohm 45sec</t>
-  </si>
-  <si>
-    <t>RT1</t>
-  </si>
-  <si>
-    <t>17.5mm</t>
-  </si>
-  <si>
-    <t>12.5x7.5</t>
-  </si>
-  <si>
-    <t>LF-1116</t>
-  </si>
-  <si>
-    <t>HYUPSIN</t>
-  </si>
-  <si>
-    <t>LINEFILTER f=120HZ L:20mH, Pin size AC10mm/BD:10mm CD:13mm Tolerance¡¾20%</t>
-  </si>
-  <si>
-    <t>LF1</t>
-  </si>
-  <si>
-    <t>21.0mm</t>
-  </si>
-  <si>
-    <t>17.0x17.0</t>
-  </si>
-  <si>
-    <t>1N4740A</t>
-  </si>
-  <si>
-    <t>Onsemi</t>
-  </si>
-  <si>
-    <t>Zener Diode Vz=10V Izsm=454mA 1W 5% DO-41</t>
-  </si>
-  <si>
-    <t>D1,D2</t>
-  </si>
-  <si>
-    <t>2.6mm</t>
-  </si>
-  <si>
-    <t>DO-204AL_DO-41</t>
-  </si>
-  <si>
-    <t>4.1x2.6</t>
-  </si>
-  <si>
-    <t>1N4744A</t>
-  </si>
-  <si>
-    <t>Zener Diode Vz=15V Izsm=304mA 1W 5% DO-41</t>
-  </si>
-  <si>
-    <t>D3,D4</t>
-  </si>
-  <si>
-    <t>GBU610</t>
-  </si>
-  <si>
-    <t>LITEON Semi</t>
-  </si>
-  <si>
-    <t>GLASS PASSIVATED BRIDGE RECTIFIERS</t>
-  </si>
-  <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>21.25mm</t>
-  </si>
-  <si>
-    <t>22.3x3.56</t>
-  </si>
-  <si>
-    <t>BR-FH1</t>
-  </si>
-  <si>
-    <t>BEE-RYONG</t>
-  </si>
-  <si>
-    <t>Fuse holder DIP</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>10.3mm</t>
-  </si>
-  <si>
-    <t>24.5x9.8</t>
-  </si>
-  <si>
-    <t>MMBT3904</t>
-  </si>
-  <si>
-    <t>NPN General-Purpose Amplifier 200mA 40V SOT-23</t>
-  </si>
-  <si>
-    <t>Q1,Q2</t>
-  </si>
-  <si>
-    <t>1.2mm</t>
-  </si>
-  <si>
-    <t>2.92x2.40</t>
-  </si>
-  <si>
-    <t>MMBT3906</t>
-  </si>
-  <si>
-    <t>PNP General-Purpose Amplifier 200mA 40V SOT-23</t>
-  </si>
-  <si>
-    <t>Q3,Q4</t>
-  </si>
-  <si>
-    <t>1.20mm</t>
-  </si>
-  <si>
-    <t>FDL100N50F</t>
-  </si>
-  <si>
-    <t>On-Semi</t>
-  </si>
-  <si>
-    <t>MOSFET N-CH 500V 100A TO-264</t>
-  </si>
-  <si>
-    <t>Q5,Q6</t>
-  </si>
-  <si>
-    <t>5.2mm</t>
-  </si>
-  <si>
-    <t>26.4x20.2</t>
-  </si>
-  <si>
-    <t>HCPL-3120-360E</t>
-  </si>
-  <si>
-    <t>AVAGO</t>
-  </si>
-  <si>
-    <t>2.5 Amp Output Current IGBT Gate Drive Optocoupler SMT</t>
-  </si>
-  <si>
-    <t>U1,U2</t>
-  </si>
-  <si>
-    <t>3.56mm</t>
-  </si>
-  <si>
-    <t>9.65x10.9</t>
-  </si>
-  <si>
-    <t>MAX3232CSE</t>
-  </si>
-  <si>
-    <t>MAXIM</t>
-  </si>
-  <si>
-    <t>3.0V to 5.5V, Low-Power, up to 1Mbps, True RS-232 Transceivers Using Four 0.1?iF External Capacitors</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
-    <t>1.75mm</t>
-  </si>
-  <si>
-    <t>MAX3232ESE</t>
-  </si>
-  <si>
-    <t>10x6.2</t>
-  </si>
-  <si>
-    <t>CAS_6-NP</t>
-  </si>
-  <si>
-    <t>CAS 6-NP</t>
-  </si>
-  <si>
-    <t>LEM</t>
-  </si>
-  <si>
-    <t>5V, 6A Current sensor</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>16mm</t>
-  </si>
-  <si>
-    <t>21.91x13.4</t>
-  </si>
-  <si>
-    <t>LM393M</t>
-  </si>
-  <si>
-    <t>On Semi</t>
-  </si>
-  <si>
-    <t>IC COMPARATOR DUAL DIFF 8-SOP</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>6.2x5.0</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>HOLE4.0MM</t>
-  </si>
-  <si>
-    <t>H1,H2,H3,H4,H5,H6</t>
-  </si>
-  <si>
-    <t>HEADER_2.54MM_1X2</t>
-  </si>
-  <si>
-    <t>HEADER_2.54mm_1x2</t>
-  </si>
-  <si>
-    <t>Anyvendor</t>
-  </si>
-  <si>
-    <t>2.54mm Pitch Pin Header 1x2 T=11.5mm</t>
-  </si>
-  <si>
-    <t>J1,J7,J8,J13,J14,J15,J16,J17</t>
-  </si>
-  <si>
-    <t>11.5mm</t>
-  </si>
-  <si>
-    <t>5.38x2.5</t>
-  </si>
-  <si>
-    <t>DSBU-9PIN</t>
-  </si>
-  <si>
-    <t>DSBU-9PIN-R/A</t>
-  </si>
-  <si>
-    <t>MOLEX</t>
-  </si>
-  <si>
-    <t>D-SUB PCB 2-row 9-pin Female Right angle</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>12.5mm</t>
-  </si>
-  <si>
-    <t>30.8x18.2</t>
-  </si>
-  <si>
-    <t>HEADER_SOCKET_20X2</t>
-  </si>
-  <si>
-    <t>HEADER_SOCKET_2.0mm_2x20</t>
-  </si>
-  <si>
-    <t>Any Vendor</t>
-  </si>
-  <si>
-    <t>2.0mm Pitch Header Socket 2x20 Straight</t>
-  </si>
-  <si>
-    <t>J9,J10</t>
-  </si>
-  <si>
-    <t>4.3mm</t>
-  </si>
-  <si>
-    <t>40.5x4.5</t>
-  </si>
-  <si>
-    <t>5273-06A</t>
-  </si>
-  <si>
-    <t>CON 6-pin, 3.96mm Pitch Throgh hole</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>13.85mm</t>
-  </si>
-  <si>
-    <t>23.0x10.2</t>
-  </si>
-  <si>
-    <t>CON2</t>
-  </si>
-  <si>
-    <t>12512WS-04B</t>
-  </si>
-  <si>
-    <t>YEONHO</t>
-  </si>
-  <si>
-    <t>CON 4-pin, Throgh hole  type</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>4.2mm</t>
-  </si>
-  <si>
-    <t>7.5x3.6</t>
-  </si>
-  <si>
-    <t>5268-04</t>
-  </si>
-  <si>
-    <t>CON Pin-4, 2.5mm pitch Right Angle</t>
-  </si>
-  <si>
-    <t>P3,P4</t>
-  </si>
-  <si>
-    <t>4.9mm</t>
-  </si>
-  <si>
-    <t>12.4x7.9</t>
-  </si>
-  <si>
-    <t>FST10-5FFM</t>
-  </si>
-  <si>
-    <t>Power Plaza</t>
-  </si>
-  <si>
-    <t>67KHz 5V, 15V AC-DC converter 0.13A@220VAC</t>
-  </si>
-  <si>
-    <t>SMPS</t>
-  </si>
-  <si>
-    <t>LM3671MF-3.3</t>
-  </si>
-  <si>
-    <t>58.0x45.0</t>
-  </si>
-  <si>
-    <t>78604/9MC</t>
-  </si>
-  <si>
-    <t>General Purpose Pulse Transformers 10mH 2:1 SMT</t>
-  </si>
-  <si>
-    <t>TX1,TX2</t>
-  </si>
-  <si>
-    <t>6.35mm</t>
-  </si>
-  <si>
-    <t>12.7x9.0</t>
-  </si>
-  <si>
-    <t>TRANSFORMER</t>
-  </si>
-  <si>
-    <t>Transformer</t>
-  </si>
-  <si>
-    <t>¼±AIAu±a</t>
-  </si>
-  <si>
-    <t>High frequency transformer 1:5</t>
-  </si>
-  <si>
-    <t>TX3</t>
-  </si>
-  <si>
-    <t>MOV-14D471K</t>
-  </si>
-  <si>
-    <t>Metal Oxide Varistor Vmax=330VAC, 14mm radial</t>
-  </si>
-  <si>
-    <t>Z1</t>
-  </si>
-  <si>
-    <t>20mm</t>
-  </si>
-  <si>
-    <t>16.5x5.4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Part Type Report1 for LF_Generator_Main_V1.0_SCH.sch on 2018-05-07 오전 12:38:14</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Design Part Type count: 36</t>
-  </si>
-  <si>
-    <t>Unit Cost</t>
-  </si>
-  <si>
-    <t>Cost</t>
-  </si>
-  <si>
-    <t>구매 Cost</t>
-  </si>
-  <si>
-    <t>필요수량</t>
-  </si>
-  <si>
-    <t>MOQ</t>
-  </si>
-  <si>
-    <t>구매수량</t>
-  </si>
-  <si>
-    <t>구매금액</t>
-  </si>
-  <si>
-    <t>ICBanQ</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>MT630V104K-15</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>L</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>T</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>18.5x6.3</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>15.0mm</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transformer_LF</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>50.8x50.0</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>TRANSFORMER_LF</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>선인전기</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>52.0mm</t>
+    <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1669,7 +1705,7 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1731,6 +1767,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1787,8 +1835,71 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="그림 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4733925" y="419100"/>
+          <a:ext cx="10906125" cy="3667125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1834,7 +1945,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1869,7 +1980,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2080,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2097,7 +2208,7 @@
   <sheetData>
     <row r="1" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -2139,28 +2250,28 @@
         <v>10</v>
       </c>
       <c r="M4" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>261</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="S4" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="T4" s="14" t="s">
         <v>267</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>268</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="T4" s="14" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
@@ -2259,51 +2370,53 @@
       <c r="S6" s="16"/>
       <c r="T6" s="9"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="22">
         <v>3</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="23" t="s">
+        <v>268</v>
+      </c>
+      <c r="H7" s="23">
+        <v>1</v>
+      </c>
+      <c r="I7" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="4">
-        <v>1</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" s="4">
+      <c r="J7" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>274</v>
+      </c>
+      <c r="L7" s="23" t="s">
+        <v>269</v>
+      </c>
+      <c r="M7" s="23">
         <v>100</v>
       </c>
-      <c r="N7" s="16"/>
-      <c r="O7" s="16"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
-      <c r="S7" s="16"/>
-      <c r="T7" s="9"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="24"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -2313,34 +2426,34 @@
         <v>4</v>
       </c>
       <c r="C8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="G8" s="16" t="s">
         <v>36</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>39</v>
       </c>
       <c r="H8" s="16">
         <v>6</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M8" s="16">
         <v>210</v>
@@ -2361,34 +2474,34 @@
         <v>5</v>
       </c>
       <c r="C9" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="16" t="s">
         <v>43</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>46</v>
       </c>
       <c r="H9" s="16">
         <v>2</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M9" s="16">
         <v>2500</v>
@@ -2409,34 +2522,34 @@
         <v>6</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H10" s="16">
         <v>9</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L10" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M10" s="16">
         <v>210</v>
@@ -2457,34 +2570,34 @@
         <v>7</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D11" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="16" t="s">
         <v>54</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>57</v>
       </c>
       <c r="H11" s="16">
         <v>2</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="M11" s="16">
         <v>210</v>
@@ -2497,53 +2610,53 @@
       <c r="S11" s="16"/>
       <c r="T11" s="9"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="12" spans="1:20" s="21" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="22">
         <v>8</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="16" t="s">
+      <c r="H12" s="23">
+        <v>2</v>
+      </c>
+      <c r="I12" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="J12" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="L12" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="16">
-        <v>2</v>
-      </c>
-      <c r="I12" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="M12" s="16">
+      <c r="M12" s="23">
         <v>1210</v>
       </c>
-      <c r="N12" s="16"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="16"/>
-      <c r="R12" s="16"/>
-      <c r="S12" s="16"/>
-      <c r="T12" s="9"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="S12" s="23"/>
+      <c r="T12" s="24"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -2553,34 +2666,34 @@
         <v>9</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F13" s="16">
         <v>300</v>
       </c>
       <c r="G13" s="16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H13" s="16">
         <v>2</v>
       </c>
       <c r="I13" s="16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K13" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L13" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M13" s="16">
         <v>10</v>
@@ -2601,34 +2714,34 @@
         <v>10</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H14" s="16">
         <v>3</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K14" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L14" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M14" s="16">
         <v>10</v>
@@ -2649,34 +2762,34 @@
         <v>11</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H15" s="16">
         <v>2</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L15" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M15" s="16">
         <v>10</v>
@@ -2697,34 +2810,34 @@
         <v>12</v>
       </c>
       <c r="C16" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="G16" s="16" t="s">
         <v>81</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>84</v>
       </c>
       <c r="H16" s="16">
         <v>2</v>
       </c>
       <c r="I16" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="J16" s="16" t="s">
-        <v>88</v>
-      </c>
       <c r="K16" s="16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L16" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M16" s="16">
         <v>10</v>
@@ -2745,34 +2858,34 @@
         <v>13</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H17" s="16">
         <v>3</v>
       </c>
       <c r="I17" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="J17" s="16" t="s">
-        <v>95</v>
-      </c>
       <c r="K17" s="16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="L17" s="16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="M17" s="16">
         <v>10</v>
@@ -2793,34 +2906,34 @@
         <v>14</v>
       </c>
       <c r="C18" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G18" s="16" t="s">
         <v>96</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" s="16" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>99</v>
       </c>
       <c r="H18" s="16">
         <v>4</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L18" s="16" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="M18" s="16">
         <v>10</v>
@@ -2841,34 +2954,34 @@
         <v>15</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G19" s="16" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="H19" s="16">
         <v>2</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L19" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M19" s="16">
         <v>10</v>
@@ -2889,34 +3002,34 @@
         <v>16</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G20" s="16" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H20" s="16">
         <v>1</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L20" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M20" s="16">
         <v>10</v>
@@ -2937,34 +3050,34 @@
         <v>17</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D21" s="16" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H21" s="16">
         <v>1</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="K21" s="16" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="L21" s="16" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M21" s="16">
         <v>10</v>
@@ -2985,34 +3098,34 @@
         <v>18</v>
       </c>
       <c r="C22" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="G22" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="G22" s="16" t="s">
-        <v>118</v>
       </c>
       <c r="H22" s="16">
         <v>1</v>
       </c>
       <c r="I22" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="J22" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="J22" s="16" t="s">
-        <v>122</v>
-      </c>
       <c r="K22" s="16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="L22" s="16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="M22" s="16"/>
       <c r="N22" s="16"/>
@@ -3031,34 +3144,34 @@
         <v>19</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H23" s="16">
         <v>1</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="L23" s="16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M23" s="16">
         <v>10</v>
@@ -3079,34 +3192,34 @@
         <v>20</v>
       </c>
       <c r="C24" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="G24" s="16" t="s">
         <v>127</v>
-      </c>
-      <c r="D24" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="E24" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="F24" s="16" t="s">
-        <v>128</v>
-      </c>
-      <c r="G24" s="16" t="s">
-        <v>130</v>
       </c>
       <c r="H24" s="16">
         <v>1</v>
       </c>
       <c r="I24" s="16" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="K24" s="16" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="L24" s="16" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="M24" s="16">
         <v>80</v>
@@ -3127,34 +3240,34 @@
         <v>21</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G25" s="16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="H25" s="16">
         <v>1</v>
       </c>
       <c r="I25" s="16" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J25" s="16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="K25" s="16" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="M25" s="16">
         <v>500</v>
@@ -3175,34 +3288,34 @@
         <v>22</v>
       </c>
       <c r="C26" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D26" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="G26" s="16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="H26" s="16">
         <v>2</v>
       </c>
       <c r="I26" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="J26" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="J26" s="16" t="s">
-        <v>146</v>
-      </c>
       <c r="K26" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L26" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="M26" s="16">
         <v>40</v>
@@ -3223,34 +3336,34 @@
         <v>23</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D27" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G27" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="H27" s="16">
         <v>2</v>
       </c>
       <c r="I27" s="16" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J27" s="16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K27" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="L27" s="16" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="M27" s="16">
         <v>40</v>
@@ -3271,34 +3384,34 @@
         <v>24</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D28" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="H28" s="16">
         <v>1</v>
       </c>
       <c r="I28" s="16" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J28" s="16" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K28" s="16" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="L28" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M28" s="16">
         <v>520</v>
@@ -3319,34 +3432,34 @@
         <v>25</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E29" s="16" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G29" s="16" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="H29" s="16">
         <v>1</v>
       </c>
       <c r="I29" s="16" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="J29" s="16" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="L29" s="16" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="M29" s="16">
         <v>70</v>
@@ -3367,34 +3480,34 @@
         <v>26</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H30" s="16">
         <v>2</v>
       </c>
       <c r="I30" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J30" s="16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L30" s="16" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="M30" s="16">
         <v>180</v>
@@ -3415,34 +3528,34 @@
         <v>27</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D31" s="16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G31" s="16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H31" s="16">
         <v>2</v>
       </c>
       <c r="I31" s="16" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="J31" s="16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K31" s="16" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="L31" s="16" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="M31" s="16">
         <v>200</v>
@@ -3463,34 +3576,34 @@
         <v>28</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H32" s="16">
         <v>2</v>
       </c>
       <c r="I32" s="16" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="J32" s="16" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="K32" s="16" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="L32" s="16" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="M32" s="16">
         <v>16900</v>
@@ -3511,34 +3624,34 @@
         <v>29</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D33" s="16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="G33" s="16" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H33" s="16">
         <v>2</v>
       </c>
       <c r="I33" s="16" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="J33" s="16" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="L33" s="16" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="M33" s="16">
         <v>3640</v>
@@ -3559,34 +3672,34 @@
         <v>30</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D34" s="16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G34" s="16" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="H34" s="16">
         <v>1</v>
       </c>
       <c r="I34" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="J34" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="J34" s="16" t="s">
-        <v>189</v>
-      </c>
       <c r="K34" s="16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="L34" s="16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="M34" s="16">
         <v>5100</v>
@@ -3607,34 +3720,34 @@
         <v>31</v>
       </c>
       <c r="C35" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="D35" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G35" s="16" t="s">
         <v>190</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="G35" s="16" t="s">
-        <v>193</v>
       </c>
       <c r="H35" s="16">
         <v>1</v>
       </c>
       <c r="I35" s="16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="J35" s="16" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="K35" s="16" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="L35" s="16" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="M35" s="16">
         <v>2850</v>
@@ -3655,34 +3768,34 @@
         <v>32</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D36" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E36" s="16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F36" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G36" s="16" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="H36" s="16">
         <v>1</v>
       </c>
       <c r="I36" s="16" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J36" s="16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="K36" s="16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="L36" s="16" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="M36" s="16">
         <v>350</v>
@@ -3703,34 +3816,34 @@
         <v>34</v>
       </c>
       <c r="C37" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="G37" s="16" t="s">
         <v>205</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="F37" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>208</v>
       </c>
       <c r="H37" s="16">
         <v>8</v>
       </c>
       <c r="I37" s="16" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J37" s="16" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K37" s="16" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="L37" s="16" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="M37" s="16">
         <v>10</v>
@@ -3751,34 +3864,34 @@
         <v>35</v>
       </c>
       <c r="C38" s="16" t="s">
+        <v>209</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="E38" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="G38" s="16" t="s">
         <v>212</v>
-      </c>
-      <c r="D38" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="E38" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="G38" s="16" t="s">
-        <v>215</v>
       </c>
       <c r="H38" s="16">
         <v>1</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J38" s="16" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="K38" s="16" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="L38" s="16" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="M38" s="16">
         <v>250</v>
@@ -3799,34 +3912,34 @@
         <v>36</v>
       </c>
       <c r="C39" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="E39" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="G39" s="16" t="s">
         <v>219</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="F39" s="16" t="s">
-        <v>220</v>
-      </c>
-      <c r="G39" s="16" t="s">
-        <v>222</v>
       </c>
       <c r="H39" s="16">
         <v>2</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="J39" s="16" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="K39" s="16" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="L39" s="16" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="M39" s="16">
         <v>1200</v>
@@ -3847,34 +3960,34 @@
         <v>37</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E40" s="16" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H40" s="16">
         <v>1</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="J40" s="16" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="K40" s="16" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="L40" s="16" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="M40" s="16">
         <v>120</v>
@@ -3895,34 +4008,34 @@
         <v>39</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="E41" s="16" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G41" s="16" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="H41" s="16">
         <v>2</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="J41" s="16" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="K41" s="16" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="L41" s="16" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
@@ -3941,34 +4054,34 @@
         <v>40</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E42" s="16" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="G42" s="16" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H42" s="16">
         <v>1</v>
       </c>
       <c r="I42" s="16" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="J42" s="16" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="K42" s="16" t="s">
         <v>18</v>
       </c>
       <c r="L42" s="16" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="M42" s="16">
         <v>20800</v>
@@ -3989,34 +4102,34 @@
         <v>41</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H43" s="16">
         <v>2</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J43" s="16" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="K43" s="16" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="L43" s="16" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="M43" s="16">
         <v>480</v>
@@ -4033,36 +4146,40 @@
       <c r="A44" t="s">
         <v>12</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="22">
         <v>42</v>
       </c>
-      <c r="C44" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="D44" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="F44" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="G44" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="H44" s="4">
+      <c r="C44" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="D44" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>275</v>
+      </c>
+      <c r="G44" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="H44" s="23">
         <v>1</v>
       </c>
-      <c r="I44" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="J44" s="4">
-        <v>0</v>
-      </c>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4">
+      <c r="I44" s="23" t="s">
+        <v>252</v>
+      </c>
+      <c r="J44" s="23" t="s">
+        <v>276</v>
+      </c>
+      <c r="K44" s="23" t="s">
+        <v>279</v>
+      </c>
+      <c r="L44" s="23" t="s">
+        <v>277</v>
+      </c>
+      <c r="M44" s="23">
         <v>45000</v>
       </c>
       <c r="N44" s="16"/>
@@ -4081,34 +4198,34 @@
         <v>43</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="E45" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="H45" s="16">
         <v>1</v>
       </c>
       <c r="I45" s="16" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="J45" s="16" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="K45" s="16" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="L45" s="16" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="M45" s="16">
         <v>500</v>
@@ -4123,40 +4240,40 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B46" s="3">
         <v>38</v>
       </c>
       <c r="C46" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G46" s="4" t="s">
         <v>231</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="H46" s="4">
         <v>1</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="K46" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="L46" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="M46" s="4">
         <v>120</v>
@@ -4171,13 +4288,13 @@
     </row>
     <row r="47" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B47" s="20">
         <v>33</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
@@ -4187,14 +4304,14 @@
         <v>6</v>
       </c>
       <c r="I47" s="17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="J47" s="17">
         <v>0</v>
       </c>
       <c r="K47" s="17"/>
       <c r="L47" s="17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
@@ -4207,7 +4324,7 @@
     </row>
     <row r="49" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -4216,4 +4333,129 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:J26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" t="s">
+        <v>271</v>
+      </c>
+      <c r="D4" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>18.5</v>
+      </c>
+      <c r="D5">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <f>B5/2</f>
+        <v>7.5</v>
+      </c>
+      <c r="C6">
+        <f>C5/2</f>
+        <v>9.25</v>
+      </c>
+      <c r="D6">
+        <f>D5/2</f>
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>12.7</v>
+      </c>
+      <c r="C14">
+        <v>45.72</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <f>B14/2</f>
+        <v>6.35</v>
+      </c>
+      <c r="C15">
+        <f>C14/2</f>
+        <v>22.86</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <f>B18/2</f>
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <f>C18/2</f>
+        <v>25.4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>270</v>
+      </c>
+      <c r="I24" t="s">
+        <v>271</v>
+      </c>
+      <c r="J24" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H25">
+        <v>7.5</v>
+      </c>
+      <c r="I25">
+        <v>10</v>
+      </c>
+      <c r="J25">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="H26">
+        <f>H25/2</f>
+        <v>3.75</v>
+      </c>
+      <c r="I26">
+        <f>I25/2</f>
+        <v>5</v>
+      </c>
+      <c r="J26">
+        <f>J25/2</f>
+        <v>2.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>